<commit_message>
Testera cuando te revientan el JOSN
</commit_message>
<xml_diff>
--- a/Plan for Hivery's Game.xlsx
+++ b/Plan for Hivery's Game.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fran/Desktop/game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fran/Documents/UC3M/game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D301B35-C750-7844-9AF5-863FF922708B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416A9EB9-9D4A-9F4F-A5EE-2CA4EF42CE64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{B6ABD925-7891-E348-BCA7-BC3A3534DCE5}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{B6ABD925-7891-E348-BCA7-BC3A3534DCE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1491,7 +1491,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">

</xml_diff>